<commit_message>
bugTest and Example test change
</commit_message>
<xml_diff>
--- a/Examples/AHP_Car_Selection/carModel_3Lvl_Excel_filledin.xlsx
+++ b/Examples/AHP_Car_Selection/carModel_3Lvl_Excel_filledin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitCODE\cdfAHPANPLib\Examples\Tutorials\AHP Car\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/GITHUB/AhpAnpLib/Examples/AHP_Car_Selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D2AD2E-9872-4717-B397-B3D9A8E8388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C128F6-5EB1-864C-9140-6E40053556E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9580" yWindow="6980" windowWidth="14620" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairwise_comp" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>GoalNode</t>
   </si>
   <si>
-    <t>Enter judgments for the paiwise comparisons in the matrix or direct values in the green cells</t>
-  </si>
-  <si>
     <t>2Criteria</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>2.2Maintenance</t>
+  </si>
+  <si>
+    <t>Enter pairwise comparisons in the white cells of the table or numerical data in the green cells. For the Direct Values column, if the smallest value is best, invert the value before entering it (e.g., $10 as =1/10) .</t>
   </si>
 </sst>
 </file>
@@ -594,54 +594,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="21" width="15.7109375" customWidth="1"/>
+    <col min="1" max="21" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -665,9 +665,9 @@
         <v>9.0908007827582696E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="10">
         <f>1/C4</f>
@@ -692,9 +692,9 @@
         <v>0.41454058202027044</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="10">
         <f>1/D4</f>
@@ -720,9 +720,9 @@
         <v>0.20363264649454607</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10">
         <f>1/E4</f>
@@ -749,9 +749,9 @@
         <v>0.29091876365760078</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="12">
         <f>SUM(B4:B7)</f>
@@ -774,51 +774,51 @@
         <v>22.916936030006017</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G9" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="12">
         <f>((MMULT(B8:E8,H4:H7)-4)/(4-1))/0.89</f>
         <v>0.11418849354492207</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="F12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -839,9 +839,9 @@
         <v>0.66242038216560506</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="10">
         <f>1/C13</f>
@@ -863,9 +863,9 @@
         <v>7.0063694267515922E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="10">
         <f>1/D13</f>
@@ -888,9 +888,9 @@
         <v>0.26751592356687898</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="12">
         <f>SUM(B13:B15)</f>
@@ -909,48 +909,48 @@
         <v>19.625</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F17" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="12">
         <f>((MMULT(B16:D16,G13:G15)-3)/(3-1))/0.52</f>
         <v>0.21741793238608551</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -968,9 +968,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="10">
         <f>1/C21</f>
@@ -989,9 +989,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="12">
         <f>SUM(B21:B22)</f>
@@ -1006,51 +1006,51 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E24" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="12">
         <f>((MMULT(B23:C23,F21:F22)-2)/(2-1))/1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="E27" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="6">
         <v>1</v>
@@ -1071,9 +1071,9 @@
         <v>0.18182182658312612</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" s="10">
         <f>1/C28</f>
@@ -1095,9 +1095,9 @@
         <v>0.27272142142545974</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="10">
         <f>1/D28</f>
@@ -1120,9 +1120,9 @@
         <v>0.54545675199141419</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="12">
         <f>SUM(B28:B30)</f>
@@ -1141,51 +1141,51 @@
         <v>10.999961001669757</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F32" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G32" s="12">
         <f>((MMULT(B31:D31,G28:G30)-3)/(3-1))/0.52</f>
         <v>-1.485644044964583E-6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="G35" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B36" s="6">
         <v>1</v>
@@ -1206,9 +1206,9 @@
         <v>0.67696440564137006</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B37" s="10">
         <f>1/C36</f>
@@ -1230,9 +1230,9 @@
         <v>0.23975822699798524</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B38" s="10">
         <f>1/D36</f>
@@ -1255,9 +1255,9 @@
         <v>8.3277367360644741E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" s="12">
         <f>SUM(B36:B38)</f>
@@ -1276,51 +1276,51 @@
         <v>17.726190476190474</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F40" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G40" s="12">
         <f>((MMULT(B39:D39,G36:G38)-3)/(3-1))/0.52</f>
         <v>0.13238105078266291</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="E43" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B44" s="6">
         <v>1</v>
@@ -1341,9 +1341,9 @@
         <v>6.3128028599601135E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" s="10">
         <f>1/C44</f>
@@ -1365,9 +1365,9 @@
         <v>0.24117485548050518</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B46" s="10">
         <f>1/D44</f>
@@ -1390,9 +1390,9 @@
         <v>0.6956971159198938</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="12">
         <f>SUM(B44:B46)</f>
@@ -1411,51 +1411,51 @@
         <v>21.561120000008998</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F48" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G48" s="12">
         <f>((MMULT(B47:D47,G44:G46)-3)/(3-1))/0.52</f>
         <v>0.29160765062619876</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="E51" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" s="6">
         <v>1</v>
@@ -1476,9 +1476,9 @@
         <v>0.22516515983160687</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B53" s="10">
         <f>1/C52</f>
@@ -1500,9 +1500,9 @@
         <v>0.33555844186206685</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B54" s="10">
         <f>1/D52</f>
@@ -1525,9 +1525,9 @@
         <v>0.43927639830632625</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55" s="12">
         <f>SUM(B52:B54)</f>
@@ -1546,9 +1546,9 @@
         <v>9.6977622793279181</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F56" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G56" s="12">
         <f>((MMULT(B55:D55,G52:G54)-3)/(3-1))/0.52</f>

</xml_diff>